<commit_message>
capex calculation revised: lifetime is replaced by payback time
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_HeatingTechnology_Cost.xlsx
+++ b/projects/test_building/input/Parameter_HeatingTechnology_Cost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247BEA62-0A15-F74A-8128-482706B15D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1665" windowWidth="17700" windowHeight="4800"/>
+    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="16">
   <si>
     <t>id_region</t>
   </si>
@@ -66,11 +66,14 @@
   <si>
     <t>exponent_om_cost</t>
   </si>
+  <si>
+    <t>payback_time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
@@ -177,23 +180,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N76" totalsRowShown="0">
-  <autoFilter ref="A1:N76"/>
-  <tableColumns count="14">
-    <tableColumn id="2" name="id_region"/>
-    <tableColumn id="4" name="id_heating_technology" dataDxfId="0"/>
-    <tableColumn id="5" name="id_heating_system_action"/>
-    <tableColumn id="6" name="unit"/>
-    <tableColumn id="7" name="multiplier_material_cost"/>
-    <tableColumn id="8" name="exponent_material_cost"/>
-    <tableColumn id="1" name="multiplier_material_share"/>
-    <tableColumn id="9" name="exponent_material_share"/>
-    <tableColumn id="3" name="learning_coefficient"/>
-    <tableColumn id="13" name="multiplier_om_cost"/>
-    <tableColumn id="14" name="exponent_om_cost"/>
-    <tableColumn id="10" name="criterion_small"/>
-    <tableColumn id="11" name="pp_index"/>
-    <tableColumn id="12" name="wages_index"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O76" totalsRowShown="0">
+  <autoFilter ref="A1:O76" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="id_region"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_heating_technology" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="id_heating_system_action"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="unit"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="multiplier_material_cost"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="exponent_material_cost"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="multiplier_material_share"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="exponent_material_share"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="learning_coefficient"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="multiplier_om_cost"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="exponent_om_cost"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="criterion_small"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="pp_index"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="wages_index"/>
+    <tableColumn id="15" xr3:uid="{D5E317A5-EE02-3948-B503-D20E2AA846DD}" name="payback_time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -461,31 +465,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="21.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,8 +532,11 @@
       <c r="N1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>9</v>
       </c>
@@ -572,8 +579,11 @@
       <c r="N2">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>9</v>
       </c>
@@ -616,8 +626,11 @@
       <c r="N3">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>9</v>
       </c>
@@ -660,8 +673,11 @@
       <c r="N4">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9</v>
       </c>
@@ -704,8 +720,11 @@
       <c r="N5">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>9</v>
       </c>
@@ -748,8 +767,11 @@
       <c r="N6">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>9</v>
       </c>
@@ -792,8 +814,11 @@
       <c r="N7">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9</v>
       </c>
@@ -836,8 +861,11 @@
       <c r="N8">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -880,8 +908,11 @@
       <c r="N9">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -924,8 +955,11 @@
       <c r="N10">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -968,8 +1002,11 @@
       <c r="N11">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1012,8 +1049,11 @@
       <c r="N12">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1056,8 +1096,11 @@
       <c r="N13">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1100,8 +1143,11 @@
       <c r="N14">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1144,8 +1190,11 @@
       <c r="N15">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1188,8 +1237,11 @@
       <c r="N16">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1232,8 +1284,11 @@
       <c r="N17">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1276,8 +1331,11 @@
       <c r="N18">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1320,8 +1378,11 @@
       <c r="N19">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
@@ -1364,8 +1425,11 @@
       <c r="N20">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9</v>
       </c>
@@ -1408,8 +1472,11 @@
       <c r="N21">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1452,8 +1519,11 @@
       <c r="N22">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>9</v>
       </c>
@@ -1496,8 +1566,11 @@
       <c r="N23">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9</v>
       </c>
@@ -1540,8 +1613,11 @@
       <c r="N24">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>9</v>
       </c>
@@ -1584,8 +1660,11 @@
       <c r="N25">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1628,8 +1707,11 @@
       <c r="N26">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1672,8 +1754,11 @@
       <c r="N27">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1716,8 +1801,11 @@
       <c r="N28">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1760,8 +1848,11 @@
       <c r="N29">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1804,8 +1895,11 @@
       <c r="N30">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>9</v>
       </c>
@@ -1848,8 +1942,11 @@
       <c r="N31">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1892,8 +1989,11 @@
       <c r="N32">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>9</v>
       </c>
@@ -1936,8 +2036,11 @@
       <c r="N33">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>9</v>
       </c>
@@ -1980,8 +2083,11 @@
       <c r="N34">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>9</v>
       </c>
@@ -2024,8 +2130,11 @@
       <c r="N35">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>9</v>
       </c>
@@ -2068,8 +2177,11 @@
       <c r="N36">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>9</v>
       </c>
@@ -2112,8 +2224,11 @@
       <c r="N37">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>9</v>
       </c>
@@ -2156,8 +2271,11 @@
       <c r="N38">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>9</v>
       </c>
@@ -2200,8 +2318,11 @@
       <c r="N39">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>9</v>
       </c>
@@ -2244,8 +2365,11 @@
       <c r="N40">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>9</v>
       </c>
@@ -2288,8 +2412,11 @@
       <c r="N41">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2332,8 +2459,11 @@
       <c r="N42">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2376,8 +2506,11 @@
       <c r="N43">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2420,8 +2553,11 @@
       <c r="N44">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2464,8 +2600,11 @@
       <c r="N45">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2508,8 +2647,11 @@
       <c r="N46">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>9</v>
       </c>
@@ -2552,8 +2694,11 @@
       <c r="N47">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>9</v>
       </c>
@@ -2596,8 +2741,11 @@
       <c r="N48">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>9</v>
       </c>
@@ -2640,8 +2788,11 @@
       <c r="N49">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>9</v>
       </c>
@@ -2684,8 +2835,11 @@
       <c r="N50">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>9</v>
       </c>
@@ -2728,8 +2882,11 @@
       <c r="N51">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>9</v>
       </c>
@@ -2772,8 +2929,11 @@
       <c r="N52">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>9</v>
       </c>
@@ -2816,8 +2976,11 @@
       <c r="N53">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>9</v>
       </c>
@@ -2860,8 +3023,11 @@
       <c r="N54">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>9</v>
       </c>
@@ -2904,8 +3070,11 @@
       <c r="N55">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>9</v>
       </c>
@@ -2948,8 +3117,11 @@
       <c r="N56">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>9</v>
       </c>
@@ -2992,8 +3164,11 @@
       <c r="N57">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>9</v>
       </c>
@@ -3036,8 +3211,11 @@
       <c r="N58">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>9</v>
       </c>
@@ -3080,8 +3258,11 @@
       <c r="N59">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>9</v>
       </c>
@@ -3124,8 +3305,11 @@
       <c r="N60">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>9</v>
       </c>
@@ -3168,8 +3352,11 @@
       <c r="N61">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>9</v>
       </c>
@@ -3212,8 +3399,11 @@
       <c r="N62">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>9</v>
       </c>
@@ -3256,8 +3446,11 @@
       <c r="N63">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>9</v>
       </c>
@@ -3300,8 +3493,11 @@
       <c r="N64">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>9</v>
       </c>
@@ -3344,8 +3540,11 @@
       <c r="N65">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>9</v>
       </c>
@@ -3388,8 +3587,11 @@
       <c r="N66">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>9</v>
       </c>
@@ -3432,8 +3634,11 @@
       <c r="N67">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>9</v>
       </c>
@@ -3476,8 +3681,11 @@
       <c r="N68">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>9</v>
       </c>
@@ -3520,8 +3728,11 @@
       <c r="N69">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>9</v>
       </c>
@@ -3564,8 +3775,11 @@
       <c r="N70">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>9</v>
       </c>
@@ -3608,8 +3822,11 @@
       <c r="N71">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>9</v>
       </c>
@@ -3652,8 +3869,11 @@
       <c r="N72">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>9</v>
       </c>
@@ -3696,8 +3916,11 @@
       <c r="N73">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>9</v>
       </c>
@@ -3740,8 +3963,11 @@
       <c r="N74">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>9</v>
       </c>
@@ -3784,8 +4010,11 @@
       <c r="N75">
         <v>0.67706708268330695</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>9</v>
       </c>
@@ -3827,6 +4056,9 @@
       </c>
       <c r="N76">
         <v>0.67706708268330695</v>
+      </c>
+      <c r="O76">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3835,397 +4067,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:C78"/>
-  <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C78" sqref="C4:C78"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C44">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C45">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C46">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C47">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C48">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C58">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C60">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C61">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C62">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C63">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C64">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C74">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C75">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C76">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C77">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C78">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="C4:C78">
-    <sortCondition ref="C4:C78"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>